<commit_message>
results extracted and saved into cp_ghiasi text files
</commit_message>
<xml_diff>
--- a/WATUM_v0.2/Dx_2017_Ghiasi_et_al_Paper03_severn_sigma02.xlsx
+++ b/WATUM_v0.2/Dx_2017_Ghiasi_et_al_Paper03_severn_sigma02.xlsx
@@ -743,12 +743,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cutive Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="40">
@@ -4797,7 +4799,7 @@
       </c>
       <c r="B2" s="44" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH("]",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
-        <v>Dx_2017_Noori_et_al_Paper02_severn.xlsx</v>
+        <v>Dx_2017_Ghiasi_et_al_Paper03_severn_sigma02.xlsx</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>

</xml_diff>